<commit_message>
gallery and topic services
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -81,13 +81,13 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>april 3 est</t>
-  </si>
-  <si>
     <t>80 hrs - ish</t>
   </si>
   <si>
     <t>april 3 actuals</t>
+  </si>
+  <si>
+    <t>estimate</t>
   </si>
 </sst>
 </file>
@@ -145,12 +145,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -488,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C28"/>
+  <dimension ref="A3:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -501,66 +503,72 @@
     <col min="3" max="3" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3">
+        <v>42464</v>
+      </c>
+      <c r="E15" s="4">
+        <v>42465</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -571,7 +579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -582,15 +590,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>10</v>
       </c>
       <c r="B18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -598,7 +612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -606,7 +620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -614,7 +628,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -622,7 +636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -630,7 +644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -638,7 +652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -646,7 +660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -654,7 +668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>19</v>
       </c>

</xml_diff>